<commit_message>
Codigo postal problem fixed
</commit_message>
<xml_diff>
--- a/Data_Prueba.xlsx
+++ b/Data_Prueba.xlsx
@@ -151,7 +151,7 @@
     <t>CORTS VALENCIANES 16 6</t>
   </si>
   <si>
-    <t>LA VALL D`UIXO</t>
+    <t>LA VALL D'UIXO</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +178,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -223,6 +230,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +599,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +666,7 @@
       <c r="E2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G2" s="3" t="s">

</xml_diff>